<commit_message>
Made it so that now height and width can be varied based on import
</commit_message>
<xml_diff>
--- a/spec/test_data/test_batch_import_with_cads.xlsx
+++ b/spec/test_data/test_batch_import_with_cads.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsellers/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsellers/code/website/spec/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="335">
   <si>
     <t>Champagne</t>
     <phoneticPr fontId="12" type="noConversion"/>
@@ -1067,6 +1067,12 @@
   </si>
   <si>
     <t>Style #</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
   </si>
 </sst>
 </file>
@@ -10860,10 +10866,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10876,7 +10882,7 @@
     <col min="7" max="7" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="41" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
         <v>332</v>
       </c>
@@ -10898,8 +10904,14 @@
       <c r="G1" s="41" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="I1" s="41" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
         <v>308</v>
       </c>
@@ -10912,8 +10924,14 @@
       <c r="F2" s="42" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="42">
+        <v>760</v>
+      </c>
+      <c r="I2" s="42">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="42" t="s">
         <v>308</v>
       </c>
@@ -10923,8 +10941,14 @@
       <c r="G3" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="42">
+        <v>100</v>
+      </c>
+      <c r="I3" s="42">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
         <v>308</v>
       </c>
@@ -10934,8 +10958,14 @@
       <c r="F4" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="42">
+        <v>760</v>
+      </c>
+      <c r="I4" s="42">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="42" t="s">
         <v>308</v>
       </c>
@@ -10945,8 +10975,14 @@
       <c r="G5" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="42">
+        <v>760</v>
+      </c>
+      <c r="I5" s="42">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
         <v>308</v>
       </c>
@@ -10956,8 +10992,14 @@
       <c r="G6" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="42">
+        <v>760</v>
+      </c>
+      <c r="I6" s="42">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
         <v>308</v>
       </c>
@@ -10975,6 +11017,12 @@
       </c>
       <c r="F7" t="s">
         <v>329</v>
+      </c>
+      <c r="H7" s="42">
+        <v>760</v>
+      </c>
+      <c r="I7" s="42">
+        <v>680</v>
       </c>
     </row>
   </sheetData>

</xml_diff>